<commit_message>
added 5 passives (armour, aoe, as, hpReg and CC), boss model, uv unwrap, rig, idle animation, consumable that pay health for knowledge
</commit_message>
<xml_diff>
--- a/Consumables.xlsx
+++ b/Consumables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -106,9 +106,6 @@
     <t>you get older slower/s</t>
   </si>
   <si>
-    <t>hp for knowledge</t>
-  </si>
-  <si>
     <t>you pay a portion of hp for knowledge</t>
   </si>
   <si>
@@ -116,12 +113,24 @@
   </si>
   <si>
     <t>you regenerate hp/second</t>
+  </si>
+  <si>
+    <t>pay hp to get some knowledge</t>
+  </si>
+  <si>
+    <t>attackSpeed</t>
+  </si>
+  <si>
+    <t>adds attacks speed to mc weapon</t>
+  </si>
+  <si>
+    <t>aoe_dmgPerSecond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,6 +299,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -325,6 +351,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -504,7 +547,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,10 +936,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -919,10 +962,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -961,9 +1004,15 @@
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -981,8 +1030,12 @@
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>

</xml_diff>

<commit_message>
player camera shake, younger and armour consumable
</commit_message>
<xml_diff>
--- a/Consumables.xlsx
+++ b/Consumables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -34,24 +34,6 @@
     <t>Iteration#3</t>
   </si>
   <si>
-    <t>heal1</t>
-  </si>
-  <si>
-    <t>heal2</t>
-  </si>
-  <si>
-    <t>heals m hp (med potency)</t>
-  </si>
-  <si>
-    <t>heals n hp (low potency)</t>
-  </si>
-  <si>
-    <t>heal3</t>
-  </si>
-  <si>
-    <t>heals x hp (high potency)</t>
-  </si>
-  <si>
     <t>bonusYoutfulness</t>
   </si>
   <si>
@@ -88,9 +70,6 @@
     <t>chance to deal a crit chance</t>
   </si>
   <si>
-    <t>getYounger</t>
-  </si>
-  <si>
     <t>you get younger when consumed</t>
   </si>
   <si>
@@ -125,12 +104,15 @@
   </si>
   <si>
     <t>aoe_dmgPerSecond</t>
+  </si>
+  <si>
+    <t>lowerAge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -155,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -196,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -205,6 +193,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,23 +290,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -351,23 +325,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,7 +504,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,15 +537,9 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -606,15 +557,9 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -632,15 +577,9 @@
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -662,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -688,10 +627,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -714,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -760,10 +699,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -782,14 +721,14 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -812,10 +751,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -854,14 +793,14 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -884,10 +823,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -910,10 +849,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -936,10 +875,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -962,10 +901,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1008,10 +947,10 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1034,7 +973,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>

</xml_diff>